<commit_message>
Fixed some bugs - simplified StartAsync
</commit_message>
<xml_diff>
--- a/Rhyous.CS6210.Hw4/Docs/Hours of Work.xlsx
+++ b/Rhyous.CS6210.Hw4/Docs/Hours of Work.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>Task</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Continued logging throughout</t>
+  </si>
+  <si>
+    <t>Debugging</t>
   </si>
 </sst>
 </file>
@@ -580,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -927,209 +930,217 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B63" s="3" t="s">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B65" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C63" s="1">
-        <f>SUM(C2:C62)</f>
-        <v>39.1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+      <c r="C65" s="1">
+        <f>SUM(C2:C64)</f>
+        <v>47.1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B66" t="s">
-        <v>44</v>
-      </c>
-      <c r="C66">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B67" t="s">
-        <v>45</v>
-      </c>
-      <c r="C67">
-        <v>0.5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
         <v>46</v>
       </c>
-      <c r="C68">
+      <c r="C70">
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B71" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
         <v>39</v>
       </c>
-      <c r="C71">
+      <c r="C73">
         <v>0.25</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B72" t="s">
-        <v>48</v>
-      </c>
-      <c r="C72">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C74">
         <v>0.25</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B75" t="s">
+      <c r="A75" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
         <v>48</v>
       </c>
-      <c r="C75">
+      <c r="C77">
         <v>0.25</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B78" t="s">
-        <v>51</v>
-      </c>
-      <c r="C78">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B79" t="s">
-        <v>54</v>
-      </c>
-      <c r="C79">
-        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C80">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
+        <v>54</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
         <v>48</v>
       </c>
-      <c r="C81">
+      <c r="C83">
         <v>0.25</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B84" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
         <v>39</v>
       </c>
-      <c r="C84">
+      <c r="C86">
         <v>0.25</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B85" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B87" t="s">
         <v>48</v>
       </c>
-      <c r="C85">
+      <c r="C87">
         <v>0.25</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B88" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
         <v>39</v>
       </c>
-      <c r="C88">
+      <c r="C90">
         <v>0.25</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B89" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B91" t="s">
         <v>48</v>
       </c>
-      <c r="C89">
+      <c r="C91">
         <v>0.25</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B92" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
         <v>39</v>
       </c>
-      <c r="C92">
+      <c r="C94">
         <v>0.25</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B93" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B95" t="s">
         <v>48</v>
       </c>
-      <c r="C93">
+      <c r="C95">
         <v>0.25</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B95" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C95" s="1">
-        <f>SUM(C65:C94)</f>
-        <v>6.4</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C97" s="1">
-        <v>2.5</v>
+        <f>SUM(C67:C96)</f>
+        <v>9.15</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B101" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C99" s="1">
-        <f>SUM(C97,C95,C63)</f>
-        <v>48</v>
+      <c r="C101" s="1">
+        <f>SUM(C99,C97,C65)</f>
+        <v>58.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>